<commit_message>
all ok, reste à verifier que on respecte tout
</commit_message>
<xml_diff>
--- a/out/Processed_RAW00.xlsx
+++ b/out/Processed_RAW00.xlsx
@@ -471,32 +471,32 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>Limite (dBµV/m)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Margin (dB)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>Polarization</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Correction (dB)</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Margin (dB)</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Overtaking (dB)</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Conformity</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Limite (dBµV/m)</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
@@ -528,31 +528,27 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>-30.75</v>
+        <v>33.25</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
           <t>Peak</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" t="n">
+        <v>64</v>
+      </c>
+      <c r="I2" t="n">
+        <v>30.75</v>
+      </c>
+      <c r="J2" t="inlineStr">
         <is>
           <t>Vertical</t>
         </is>
       </c>
-      <c r="I2" t="n">
+      <c r="K2" t="n">
         <v>9.92</v>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="L2" t="inlineStr">
         <is>
           <t>-</t>
@@ -560,7 +556,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>OK</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -592,31 +588,27 @@
         <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>-35.85</v>
+        <v>22.15</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
           <t>Peak</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H3" t="n">
+        <v>58</v>
+      </c>
+      <c r="I3" t="n">
+        <v>35.85</v>
+      </c>
+      <c r="J3" t="inlineStr">
         <is>
           <t>Vertical</t>
         </is>
       </c>
-      <c r="I3" t="n">
+      <c r="K3" t="n">
         <v>10.29</v>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>-</t>
@@ -624,7 +616,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>OK</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -646,7 +638,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Peak</t>
+          <t>Q-Peak</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -656,31 +648,27 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>-19.61</v>
+        <v>31.39</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Peak</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
+          <t>Q-Peak</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>51</v>
+      </c>
+      <c r="I4" t="n">
+        <v>19.61</v>
+      </c>
+      <c r="J4" t="inlineStr">
         <is>
           <t>Vertical</t>
         </is>
       </c>
-      <c r="I4" t="n">
+      <c r="K4" t="n">
         <v>9.92</v>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="L4" t="inlineStr">
         <is>
           <t>-</t>
@@ -688,7 +676,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>OK</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -710,7 +698,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Peak</t>
+          <t>Q-Peak</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -720,31 +708,27 @@
         <v>2</v>
       </c>
       <c r="F5" t="n">
-        <v>-28.95</v>
+        <v>16.05</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Peak</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
+          <t>Q-Peak</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>45</v>
+      </c>
+      <c r="I5" t="n">
+        <v>28.95</v>
+      </c>
+      <c r="J5" t="inlineStr">
         <is>
           <t>Vertical</t>
         </is>
       </c>
-      <c r="I5" t="n">
+      <c r="K5" t="n">
         <v>10.29</v>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>-</t>
@@ -752,7 +736,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>OK</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -784,31 +768,27 @@
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>-17.75</v>
+        <v>33.25</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
           <t>Peak</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="H6" t="n">
+        <v>51</v>
+      </c>
+      <c r="I6" t="n">
+        <v>17.75</v>
+      </c>
+      <c r="J6" t="inlineStr">
         <is>
           <t>Vertical</t>
         </is>
       </c>
-      <c r="I6" t="n">
+      <c r="K6" t="n">
         <v>9.92</v>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>-</t>
@@ -816,7 +796,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>OK</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -848,31 +828,27 @@
         <v>2</v>
       </c>
       <c r="F7" t="n">
-        <v>-22.85</v>
+        <v>22.15</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
           <t>Peak</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H7" t="n">
+        <v>45</v>
+      </c>
+      <c r="I7" t="n">
+        <v>22.85</v>
+      </c>
+      <c r="J7" t="inlineStr">
         <is>
           <t>Vertical</t>
         </is>
       </c>
-      <c r="I7" t="n">
+      <c r="K7" t="n">
         <v>10.29</v>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>-</t>
@@ -880,7 +856,7 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>OK</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -912,36 +888,36 @@
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>-25.65</v>
+        <v>18.35</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
           <t>CISPR.AVG</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="H8" t="n">
+        <v>44</v>
+      </c>
+      <c r="I8" t="n">
+        <v>25.65</v>
+      </c>
+      <c r="J8" t="inlineStr">
         <is>
           <t>Vertical</t>
         </is>
       </c>
-      <c r="I8" t="n">
+      <c r="K8" t="n">
         <v>9.92</v>
       </c>
-      <c r="J8" t="n">
-        <v>69.65000000000001</v>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="L8" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
           <t>OK</t>
         </is>
-      </c>
-      <c r="M8" t="n">
-        <v>44</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -972,36 +948,36 @@
         <v>2</v>
       </c>
       <c r="F9" t="n">
-        <v>-23.43</v>
+        <v>4.57</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
           <t>CISPR.AVG</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="H9" t="n">
+        <v>28</v>
+      </c>
+      <c r="I9" t="n">
+        <v>23.43</v>
+      </c>
+      <c r="J9" t="inlineStr">
         <is>
           <t>Vertical</t>
         </is>
       </c>
-      <c r="I9" t="n">
+      <c r="K9" t="n">
         <v>10.29</v>
       </c>
-      <c r="J9" t="n">
-        <v>51.43</v>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="L9" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
           <t>OK</t>
         </is>
-      </c>
-      <c r="M9" t="n">
-        <v>28</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>

</xml_diff>